<commit_message>
Se cambia el tipo de datos para propiedad documentID y verififcationDigit e los CRM´s
</commit_message>
<xml_diff>
--- a/public/DownloadExcels/Sedes.xlsx
+++ b/public/DownloadExcels/Sedes.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Mario\Desktop\Ecopcion Definitivo\ecopFront\public\DownloadExcels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos Reyes\OneDrive - Top Drive Group\Escritorio\CARLOS\Ecop\ecopFront\public\DownloadExcels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B2ED31-8029-4ECA-8F90-50A845A42DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F75C2A3-6DE5-483E-9E63-66F06A71D8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEDES" sheetId="1" r:id="rId1"/>
-    <sheet name="Lista desplegable" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="Lista desplegable" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -4127,7 +4127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -17631,8 +17631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J1117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>